<commit_message>
Minor updates to colour and change view implementation
</commit_message>
<xml_diff>
--- a/Planets/planetData.xlsx
+++ b/Planets/planetData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danda\Documents\School Work\NUS\Semester 2\Computational Methods\main\Planets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFC26657-D3B4-4C24-82A3-74472EB3B33E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17357C16-1875-4539-A8BC-8E2CF1A9A29C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10028" xr2:uid="{9F7D8285-D4B4-40F2-8B52-266A6ED0BEAB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Perihelion</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Radius km</t>
   </si>
   <si>
-    <t>distToSun [10^9 m]</t>
-  </si>
-  <si>
     <t>Sidereal Period [days]</t>
   </si>
   <si>
@@ -75,6 +72,24 @@
   </si>
   <si>
     <t>Pluto</t>
+  </si>
+  <si>
+    <t>Phobos</t>
+  </si>
+  <si>
+    <t>distToParent [10^9 m]</t>
+  </si>
+  <si>
+    <t>10.6*10^15</t>
+  </si>
+  <si>
+    <t>Deimos</t>
+  </si>
+  <si>
+    <t>1.4762×10^15</t>
+  </si>
+  <si>
+    <t>Moon</t>
   </si>
 </sst>
 </file>
@@ -428,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C26FC4-52E8-4344-BDF3-E08080642836}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -442,7 +457,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -454,10 +469,10 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -505,7 +520,7 @@
         <v>108.9</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G20" si="0">(E4+F4)/2</f>
+        <f t="shared" ref="G4:G13" si="0">(E4+F4)/2</f>
         <v>108.2</v>
       </c>
       <c r="H4">
@@ -514,7 +529,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>5.9722999999999997</v>
@@ -538,7 +553,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0.64171</v>
@@ -562,7 +577,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1898.19</v>
@@ -586,7 +601,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>568.34</v>
@@ -610,7 +625,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>86.813000000000002</v>
@@ -634,7 +649,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>102.413</v>
@@ -658,7 +673,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1.303E-2</v>
@@ -678,6 +693,63 @@
       </c>
       <c r="H11" s="1">
         <v>90560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>7.3459999999999998E-2</v>
+      </c>
+      <c r="D13">
+        <v>1738.1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.36330000000000001</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.40550000000000003</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.38440000000000002</v>
+      </c>
+      <c r="H13" s="1">
+        <v>27.3217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>9375000</v>
+      </c>
+      <c r="H14">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>